<commit_message>
Ultimos cambios en el libro
</commit_message>
<xml_diff>
--- a/Presentacion/Estado del arte - resumido.xlsx
+++ b/Presentacion/Estado del arte - resumido.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Parte 1" sheetId="1" r:id="rId1"/>
@@ -26,18 +26,6 @@
     <t>RESULTADOS</t>
   </si>
   <si>
-    <t>Demanda diaria de productos alimenticios perecederos [Huber2017]</t>
-  </si>
-  <si>
-    <t>Demanda anual de gas natural para la ciudad de Sakarya en Turquía [#Akpinar2016]</t>
-  </si>
-  <si>
-    <t>Pronóstico a corto plazo de la llegada de turistas en la ciudad de Montenegro [#Bigovic2012]</t>
-  </si>
-  <si>
-    <t>Demanda en una cadena farmacéutica minorista (retail) Apollo Pharmacy que cuenta con 70 puntos de venta en la India [#LakshmiAnusha2014]</t>
-  </si>
-  <si>
     <t>• ARIMA multivariante.</t>
   </si>
   <si>
@@ -70,12 +58,6 @@
     <t xml:space="preserve">• Para productos de demanda constante el método de Promedio Móvil tiene una mayor precisión.
 • Para productos estacionales el Suavizamiento Exponencial de Winters tiene mejor pronóstico
 </t>
-  </si>
-  <si>
-    <t>Demanda de agua urbana en la ciudad de Montreal [#Mouatadid2016]</t>
-  </si>
-  <si>
-    <t>Demanda de estilos nunca antes vendidos y buscar un algoritmo que optimice combinaciones de precios [#Ferreira2015]</t>
   </si>
   <si>
     <t>• Artificial Neural Network (ANN)
@@ -96,9 +78,6 @@
 • Los ingresos del grupo de prueba aumentaron en aproximadamente 9.7%.</t>
   </si>
   <si>
-    <t>Demanda del petróleo crudo importado (Imported Crude Oil - ICO) en Taiwán [#HybridSoft2014]</t>
-  </si>
-  <si>
     <t>• Multiple Linear Regression (MLR),
 • Support Vector Regression (SVR),
 • Artificial Neural Networks (ANN),
@@ -111,6 +90,27 @@
   <si>
     <t>• Los enfoques híbridos propuestos son más precisos que los de una sola etapa. 
 • Los enfoques híbridos son capaces de predecir con mayor precisión la demanda de petróleo crudo.</t>
+  </si>
+  <si>
+    <t>Demanda diaria de productos alimenticios perecederos [HGS17]</t>
+  </si>
+  <si>
+    <t>Demanda anual de gas natural para la ciudad de Sakarya en Turquía [AY16]</t>
+  </si>
+  <si>
+    <t>Pronóstico a corto plazo de la llegada de turistas en la ciudad de Montenegro [Big12]</t>
+  </si>
+  <si>
+    <t>Demanda en una cadena farmacéutica minorista (retail) Apollo Pharmacy que cuenta con 70 puntos de venta en la India [LAAS14]</t>
+  </si>
+  <si>
+    <t>Demanda de agua urbana en la ciudad de Montreal [MA16]</t>
+  </si>
+  <si>
+    <t>Demanda de estilos nunca antes vendidos y buscar un algoritmo que optimice combinaciones de precios [FLSL15]</t>
+  </si>
+  <si>
+    <t>Demanda del petróleo crudo importado en Taiwán [SLH14]</t>
   </si>
 </sst>
 </file>
@@ -146,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -154,23 +154,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -188,6 +176,18 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -203,28 +203,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:C5" totalsRowShown="0" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:C5" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
   <autoFilter ref="A1:C5">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" name="PROBLEMA" dataDxfId="8"/>
-    <tableColumn id="2" name="TÉCNICA DE SOLUCIÓN" dataDxfId="7"/>
-    <tableColumn id="3" name="RESULTADOS" dataDxfId="6"/>
+    <tableColumn id="1" name="PROBLEMA" dataDxfId="4"/>
+    <tableColumn id="2" name="TÉCNICA DE SOLUCIÓN" dataDxfId="3"/>
+    <tableColumn id="3" name="RESULTADOS" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla24" displayName="Tabla24" ref="A1:C4" totalsRowShown="0" headerRowDxfId="4" dataDxfId="0">
-  <autoFilter ref="A1:C4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla24" displayName="Tabla24" ref="A1:C4" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:C4">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+  </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" name="PROBLEMA" dataDxfId="3"/>
-    <tableColumn id="2" name="TÉCNICA DE SOLUCIÓN" dataDxfId="2"/>
-    <tableColumn id="3" name="RESULTADOS" dataDxfId="1"/>
+    <tableColumn id="1" name="PROBLEMA" dataDxfId="7"/>
+    <tableColumn id="2" name="TÉCNICA DE SOLUCIÓN" dataDxfId="6"/>
+    <tableColumn id="3" name="RESULTADOS" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -519,70 +523,70 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="5" spans="1:3" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -598,7 +602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
@@ -622,35 +626,35 @@
     </row>
     <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>